<commit_message>
Updated 90- and 30-day mortality.
</commit_message>
<xml_diff>
--- a/GMADD_study_metadata.xlsx
+++ b/GMADD_study_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpanz\Documents\Theis_Lab_Analysis\Fecal_Chopra\Updated_Run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E50523B-4ED3-4349-AF52-0B1AB868FE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3FBFAD-FDBD-476A-ACA8-4C6B95218314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="343">
   <si>
     <t>Age</t>
   </si>
@@ -1259,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1410,11 +1410,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1731,9 +1727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="AS44" sqref="AS44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8407,7 +8403,7 @@
       <c r="E35" s="42">
         <v>90</v>
       </c>
-      <c r="F35" s="56">
+      <c r="F35" s="42">
         <v>22</v>
       </c>
       <c r="G35" s="42">
@@ -9874,11 +9870,11 @@
       <c r="AQ42" s="42">
         <v>0</v>
       </c>
-      <c r="AR42" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="AS42" s="42" t="s">
-        <v>104</v>
+      <c r="AR42" s="42">
+        <v>0</v>
+      </c>
+      <c r="AS42" s="42">
+        <v>0</v>
       </c>
       <c r="AT42" s="42">
         <v>0</v>
@@ -10072,8 +10068,8 @@
       <c r="AR43" s="45">
         <v>0</v>
       </c>
-      <c r="AS43" s="42" t="s">
-        <v>104</v>
+      <c r="AS43" s="42">
+        <v>0</v>
       </c>
       <c r="AT43" s="45">
         <v>1</v>
@@ -10265,8 +10261,8 @@
       <c r="AR44" s="45">
         <v>0</v>
       </c>
-      <c r="AS44" s="42" t="s">
-        <v>104</v>
+      <c r="AS44" s="42">
+        <v>0</v>
       </c>
       <c r="AT44" s="45">
         <v>1</v>
@@ -10458,8 +10454,8 @@
       <c r="AR45" s="45">
         <v>0</v>
       </c>
-      <c r="AS45" s="45" t="s">
-        <v>104</v>
+      <c r="AS45" s="42">
+        <v>0</v>
       </c>
       <c r="AT45" s="45">
         <v>0</v>
@@ -10653,8 +10649,8 @@
       <c r="AR46" s="51">
         <v>0</v>
       </c>
-      <c r="AS46" s="51" t="s">
-        <v>104</v>
+      <c r="AS46" s="42">
+        <v>0</v>
       </c>
       <c r="AT46" s="51">
         <v>1</v>
@@ -11035,7 +11031,7 @@
       <c r="R2" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="56" t="s">
         <v>338</v>
       </c>
       <c r="T2" s="31" t="s">
@@ -11056,7 +11052,7 @@
       <c r="Y2" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="56" t="s">
         <v>339</v>
       </c>
       <c r="AA2" s="31" t="s">
@@ -11137,31 +11133,31 @@
       <c r="AZ2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="BA2" s="58" t="s">
+      <c r="BA2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BB2" s="58" t="s">
+      <c r="BB2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BC2" s="58" t="s">
+      <c r="BC2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BD2" s="58" t="s">
+      <c r="BD2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BE2" s="58" t="s">
+      <c r="BE2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BF2" s="58" t="s">
+      <c r="BF2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BG2" s="58" t="s">
+      <c r="BG2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BH2" s="58" t="s">
+      <c r="BH2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="BI2" s="58" t="s">
+      <c r="BI2" s="31" t="s">
         <v>340</v>
       </c>
       <c r="BJ2" s="31" t="s">
@@ -11204,7 +11200,7 @@
       <c r="R3" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="S3" s="58"/>
+      <c r="S3" s="31"/>
       <c r="T3" s="31" t="s">
         <v>175</v>
       </c>
@@ -11223,7 +11219,7 @@
       <c r="Y3" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="Z3" s="58"/>
+      <c r="Z3" s="31"/>
       <c r="AA3" s="31" t="s">
         <v>173</v>
       </c>
@@ -11298,31 +11294,31 @@
       </c>
       <c r="AY3" s="31"/>
       <c r="AZ3" s="28"/>
-      <c r="BA3" s="58" t="s">
+      <c r="BA3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BB3" s="58" t="s">
+      <c r="BB3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BC3" s="58" t="s">
+      <c r="BC3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BD3" s="58" t="s">
+      <c r="BD3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BE3" s="58" t="s">
+      <c r="BE3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BF3" s="58" t="s">
+      <c r="BF3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BG3" s="58" t="s">
+      <c r="BG3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BH3" s="58" t="s">
+      <c r="BH3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="BI3" s="58" t="s">
+      <c r="BI3" s="31" t="s">
         <v>341</v>
       </c>
       <c r="BJ3" s="31"/>
@@ -11355,7 +11351,7 @@
       </c>
       <c r="Q4" s="31"/>
       <c r="R4" s="31"/>
-      <c r="S4" s="58"/>
+      <c r="S4" s="31"/>
       <c r="T4" s="31" t="s">
         <v>184</v>
       </c>
@@ -11370,7 +11366,7 @@
       <c r="Y4" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="Z4" s="58"/>
+      <c r="Z4" s="31"/>
       <c r="AA4" s="31"/>
       <c r="AB4" s="31"/>
       <c r="AC4" s="31" t="s">
@@ -11405,31 +11401,31 @@
       <c r="AX4" s="31"/>
       <c r="AY4" s="31"/>
       <c r="AZ4" s="28"/>
-      <c r="BA4" s="58" t="s">
+      <c r="BA4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BB4" s="58" t="s">
+      <c r="BB4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BC4" s="58" t="s">
+      <c r="BC4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BD4" s="58" t="s">
+      <c r="BD4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BE4" s="58" t="s">
+      <c r="BE4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BF4" s="58" t="s">
+      <c r="BF4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BG4" s="58" t="s">
+      <c r="BG4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BH4" s="58" t="s">
+      <c r="BH4" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="BI4" s="58" t="s">
+      <c r="BI4" s="31" t="s">
         <v>342</v>
       </c>
       <c r="BJ4" s="31"/>
@@ -11460,7 +11456,7 @@
       </c>
       <c r="Q5" s="31"/>
       <c r="R5" s="31"/>
-      <c r="S5" s="58"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="31" t="s">
         <v>194</v>
       </c>
@@ -11471,7 +11467,7 @@
       <c r="W5" s="31"/>
       <c r="X5" s="31"/>
       <c r="Y5" s="31"/>
-      <c r="Z5" s="58"/>
+      <c r="Z5" s="31"/>
       <c r="AA5" s="31"/>
       <c r="AB5" s="31"/>
       <c r="AC5" s="31"/>
@@ -11498,15 +11494,15 @@
       <c r="AX5" s="31"/>
       <c r="AY5" s="31"/>
       <c r="AZ5" s="28"/>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
-      <c r="BC5" s="58"/>
-      <c r="BD5" s="58"/>
-      <c r="BE5" s="58"/>
-      <c r="BF5" s="58"/>
-      <c r="BG5" s="58"/>
-      <c r="BH5" s="58"/>
-      <c r="BI5" s="58"/>
+      <c r="BA5" s="31"/>
+      <c r="BB5" s="31"/>
+      <c r="BC5" s="31"/>
+      <c r="BD5" s="31"/>
+      <c r="BE5" s="31"/>
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="31"/>
+      <c r="BH5" s="31"/>
+      <c r="BI5" s="31"/>
       <c r="BJ5" s="31"/>
       <c r="BK5" s="31"/>
     </row>
@@ -11531,7 +11527,7 @@
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
       <c r="R6" s="31"/>
-      <c r="S6" s="58"/>
+      <c r="S6" s="31"/>
       <c r="T6" s="31" t="s">
         <v>196</v>
       </c>
@@ -11542,7 +11538,7 @@
       <c r="W6" s="31"/>
       <c r="X6" s="31"/>
       <c r="Y6" s="31"/>
-      <c r="Z6" s="58"/>
+      <c r="Z6" s="31"/>
       <c r="AA6" s="31"/>
       <c r="AB6" s="31"/>
       <c r="AC6" s="31"/>
@@ -11569,15 +11565,15 @@
       <c r="AX6" s="31"/>
       <c r="AY6" s="31"/>
       <c r="AZ6" s="28"/>
-      <c r="BA6" s="58"/>
-      <c r="BB6" s="58"/>
-      <c r="BC6" s="58"/>
-      <c r="BD6" s="58"/>
-      <c r="BE6" s="58"/>
-      <c r="BF6" s="58"/>
-      <c r="BG6" s="58"/>
-      <c r="BH6" s="58"/>
-      <c r="BI6" s="58"/>
+      <c r="BA6" s="31"/>
+      <c r="BB6" s="31"/>
+      <c r="BC6" s="31"/>
+      <c r="BD6" s="31"/>
+      <c r="BE6" s="31"/>
+      <c r="BF6" s="31"/>
+      <c r="BG6" s="31"/>
+      <c r="BH6" s="31"/>
+      <c r="BI6" s="31"/>
       <c r="BJ6" s="31"/>
       <c r="BK6" s="31"/>
     </row>
@@ -11600,7 +11596,7 @@
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
       <c r="R7" s="31"/>
-      <c r="S7" s="58"/>
+      <c r="S7" s="31"/>
       <c r="T7" s="31" t="s">
         <v>197</v>
       </c>
@@ -11611,7 +11607,7 @@
       <c r="W7" s="31"/>
       <c r="X7" s="31"/>
       <c r="Y7" s="31"/>
-      <c r="Z7" s="58"/>
+      <c r="Z7" s="31"/>
       <c r="AA7" s="31"/>
       <c r="AB7" s="31"/>
       <c r="AC7" s="31"/>
@@ -11638,15 +11634,15 @@
       <c r="AX7" s="31"/>
       <c r="AY7" s="31"/>
       <c r="AZ7" s="28"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="58"/>
-      <c r="BF7" s="58"/>
-      <c r="BG7" s="58"/>
-      <c r="BH7" s="58"/>
-      <c r="BI7" s="58"/>
+      <c r="BA7" s="31"/>
+      <c r="BB7" s="31"/>
+      <c r="BC7" s="31"/>
+      <c r="BD7" s="31"/>
+      <c r="BE7" s="31"/>
+      <c r="BF7" s="31"/>
+      <c r="BG7" s="31"/>
+      <c r="BH7" s="31"/>
+      <c r="BI7" s="31"/>
       <c r="BJ7" s="31"/>
       <c r="BK7" s="31"/>
     </row>
@@ -11669,7 +11665,7 @@
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
       <c r="R8" s="31"/>
-      <c r="S8" s="58"/>
+      <c r="S8" s="31"/>
       <c r="T8" s="31" t="s">
         <v>198</v>
       </c>
@@ -11680,7 +11676,7 @@
       <c r="W8" s="31"/>
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
-      <c r="Z8" s="58"/>
+      <c r="Z8" s="31"/>
       <c r="AA8" s="31"/>
       <c r="AB8" s="31"/>
       <c r="AC8" s="31"/>
@@ -11707,15 +11703,15 @@
       <c r="AX8" s="31"/>
       <c r="AY8" s="31"/>
       <c r="AZ8" s="28"/>
-      <c r="BA8" s="58"/>
-      <c r="BB8" s="58"/>
-      <c r="BC8" s="58"/>
-      <c r="BD8" s="58"/>
-      <c r="BE8" s="58"/>
-      <c r="BF8" s="58"/>
-      <c r="BG8" s="58"/>
-      <c r="BH8" s="58"/>
-      <c r="BI8" s="58"/>
+      <c r="BA8" s="31"/>
+      <c r="BB8" s="31"/>
+      <c r="BC8" s="31"/>
+      <c r="BD8" s="31"/>
+      <c r="BE8" s="31"/>
+      <c r="BF8" s="31"/>
+      <c r="BG8" s="31"/>
+      <c r="BH8" s="31"/>
+      <c r="BI8" s="31"/>
       <c r="BJ8" s="31"/>
       <c r="BK8" s="31"/>
     </row>
@@ -11738,7 +11734,7 @@
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
       <c r="R9" s="31"/>
-      <c r="S9" s="58"/>
+      <c r="S9" s="31"/>
       <c r="T9" s="31" t="s">
         <v>199</v>
       </c>
@@ -11749,7 +11745,7 @@
       <c r="W9" s="31"/>
       <c r="X9" s="31"/>
       <c r="Y9" s="31"/>
-      <c r="Z9" s="58"/>
+      <c r="Z9" s="31"/>
       <c r="AA9" s="31"/>
       <c r="AB9" s="31"/>
       <c r="AC9" s="31"/>
@@ -11776,15 +11772,15 @@
       <c r="AX9" s="31"/>
       <c r="AY9" s="31"/>
       <c r="AZ9" s="28"/>
-      <c r="BA9" s="58"/>
-      <c r="BB9" s="58"/>
-      <c r="BC9" s="58"/>
-      <c r="BD9" s="58"/>
-      <c r="BE9" s="58"/>
-      <c r="BF9" s="58"/>
-      <c r="BG9" s="58"/>
-      <c r="BH9" s="58"/>
-      <c r="BI9" s="58"/>
+      <c r="BA9" s="31"/>
+      <c r="BB9" s="31"/>
+      <c r="BC9" s="31"/>
+      <c r="BD9" s="31"/>
+      <c r="BE9" s="31"/>
+      <c r="BF9" s="31"/>
+      <c r="BG9" s="31"/>
+      <c r="BH9" s="31"/>
+      <c r="BI9" s="31"/>
       <c r="BJ9" s="31"/>
       <c r="BK9" s="31"/>
     </row>
@@ -11807,7 +11803,7 @@
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
-      <c r="S10" s="58"/>
+      <c r="S10" s="31"/>
       <c r="T10" s="31"/>
       <c r="U10" s="37" t="s">
         <v>275</v>
@@ -11816,7 +11812,7 @@
       <c r="W10" s="31"/>
       <c r="X10" s="31"/>
       <c r="Y10" s="31"/>
-      <c r="Z10" s="58"/>
+      <c r="Z10" s="31"/>
       <c r="AA10" s="31"/>
       <c r="AB10" s="31"/>
       <c r="AC10" s="31"/>
@@ -11843,15 +11839,15 @@
       <c r="AX10" s="31"/>
       <c r="AY10" s="31"/>
       <c r="AZ10" s="28"/>
-      <c r="BA10" s="58"/>
-      <c r="BB10" s="58"/>
-      <c r="BC10" s="58"/>
-      <c r="BD10" s="58"/>
-      <c r="BE10" s="58"/>
-      <c r="BF10" s="58"/>
-      <c r="BG10" s="58"/>
-      <c r="BH10" s="58"/>
-      <c r="BI10" s="58"/>
+      <c r="BA10" s="31"/>
+      <c r="BB10" s="31"/>
+      <c r="BC10" s="31"/>
+      <c r="BD10" s="31"/>
+      <c r="BE10" s="31"/>
+      <c r="BF10" s="31"/>
+      <c r="BG10" s="31"/>
+      <c r="BH10" s="31"/>
+      <c r="BI10" s="31"/>
       <c r="BJ10" s="31"/>
       <c r="BK10" s="31"/>
     </row>
@@ -11874,7 +11870,7 @@
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
       <c r="R11" s="31"/>
-      <c r="S11" s="58"/>
+      <c r="S11" s="31"/>
       <c r="T11" s="31"/>
       <c r="U11" s="38" t="s">
         <v>276</v>
@@ -11883,7 +11879,7 @@
       <c r="W11" s="31"/>
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
-      <c r="Z11" s="58"/>
+      <c r="Z11" s="31"/>
       <c r="AA11" s="31"/>
       <c r="AB11" s="31"/>
       <c r="AC11" s="31"/>
@@ -11910,15 +11906,15 @@
       <c r="AX11" s="31"/>
       <c r="AY11" s="31"/>
       <c r="AZ11" s="28"/>
-      <c r="BA11" s="58"/>
-      <c r="BB11" s="58"/>
-      <c r="BC11" s="58"/>
-      <c r="BD11" s="58"/>
-      <c r="BE11" s="58"/>
-      <c r="BF11" s="58"/>
-      <c r="BG11" s="58"/>
-      <c r="BH11" s="58"/>
-      <c r="BI11" s="58"/>
+      <c r="BA11" s="31"/>
+      <c r="BB11" s="31"/>
+      <c r="BC11" s="31"/>
+      <c r="BD11" s="31"/>
+      <c r="BE11" s="31"/>
+      <c r="BF11" s="31"/>
+      <c r="BG11" s="31"/>
+      <c r="BH11" s="31"/>
+      <c r="BI11" s="31"/>
       <c r="BJ11" s="31"/>
       <c r="BK11" s="31"/>
     </row>
@@ -11941,7 +11937,7 @@
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
-      <c r="S12" s="58"/>
+      <c r="S12" s="31"/>
       <c r="T12" s="31"/>
       <c r="U12" s="39" t="s">
         <v>277</v>
@@ -11950,7 +11946,7 @@
       <c r="W12" s="31"/>
       <c r="X12" s="31"/>
       <c r="Y12" s="31"/>
-      <c r="Z12" s="58"/>
+      <c r="Z12" s="31"/>
       <c r="AA12" s="31"/>
       <c r="AB12" s="31"/>
       <c r="AC12" s="31"/>
@@ -11977,15 +11973,15 @@
       <c r="AX12" s="31"/>
       <c r="AY12" s="31"/>
       <c r="AZ12" s="28"/>
-      <c r="BA12" s="58"/>
-      <c r="BB12" s="58"/>
-      <c r="BC12" s="58"/>
-      <c r="BD12" s="58"/>
-      <c r="BE12" s="58"/>
-      <c r="BF12" s="58"/>
-      <c r="BG12" s="58"/>
-      <c r="BH12" s="58"/>
-      <c r="BI12" s="58"/>
+      <c r="BA12" s="31"/>
+      <c r="BB12" s="31"/>
+      <c r="BC12" s="31"/>
+      <c r="BD12" s="31"/>
+      <c r="BE12" s="31"/>
+      <c r="BF12" s="31"/>
+      <c r="BG12" s="31"/>
+      <c r="BH12" s="31"/>
+      <c r="BI12" s="31"/>
       <c r="BJ12" s="31"/>
       <c r="BK12" s="31"/>
     </row>
@@ -12008,7 +12004,7 @@
       <c r="P13" s="31"/>
       <c r="Q13" s="31"/>
       <c r="R13" s="31"/>
-      <c r="S13" s="58"/>
+      <c r="S13" s="31"/>
       <c r="T13" s="31"/>
       <c r="U13" s="40" t="s">
         <v>278</v>
@@ -12017,7 +12013,7 @@
       <c r="W13" s="31"/>
       <c r="X13" s="31"/>
       <c r="Y13" s="31"/>
-      <c r="Z13" s="58"/>
+      <c r="Z13" s="31"/>
       <c r="AA13" s="31"/>
       <c r="AB13" s="31"/>
       <c r="AC13" s="31"/>
@@ -12044,15 +12040,15 @@
       <c r="AX13" s="31"/>
       <c r="AY13" s="31"/>
       <c r="AZ13" s="28"/>
-      <c r="BA13" s="58"/>
-      <c r="BB13" s="58"/>
-      <c r="BC13" s="58"/>
-      <c r="BD13" s="58"/>
-      <c r="BE13" s="58"/>
-      <c r="BF13" s="58"/>
-      <c r="BG13" s="58"/>
-      <c r="BH13" s="58"/>
-      <c r="BI13" s="58"/>
+      <c r="BA13" s="31"/>
+      <c r="BB13" s="31"/>
+      <c r="BC13" s="31"/>
+      <c r="BD13" s="31"/>
+      <c r="BE13" s="31"/>
+      <c r="BF13" s="31"/>
+      <c r="BG13" s="31"/>
+      <c r="BH13" s="31"/>
+      <c r="BI13" s="31"/>
       <c r="BJ13" s="31"/>
       <c r="BK13" s="31"/>
     </row>
@@ -12075,7 +12071,7 @@
       <c r="P14" s="31"/>
       <c r="Q14" s="31"/>
       <c r="R14" s="41"/>
-      <c r="S14" s="58"/>
+      <c r="S14" s="31"/>
       <c r="T14" s="31"/>
       <c r="U14" s="28" t="s">
         <v>279</v>
@@ -12084,7 +12080,7 @@
       <c r="W14" s="31"/>
       <c r="X14" s="31"/>
       <c r="Y14" s="31"/>
-      <c r="Z14" s="58"/>
+      <c r="Z14" s="31"/>
       <c r="AA14" s="31"/>
       <c r="AB14" s="31"/>
       <c r="AC14" s="31"/>
@@ -12111,15 +12107,15 @@
       <c r="AX14" s="31"/>
       <c r="AY14" s="31"/>
       <c r="AZ14" s="28"/>
-      <c r="BA14" s="58"/>
-      <c r="BB14" s="58"/>
-      <c r="BC14" s="58"/>
-      <c r="BD14" s="58"/>
-      <c r="BE14" s="58"/>
-      <c r="BF14" s="58"/>
-      <c r="BG14" s="58"/>
-      <c r="BH14" s="58"/>
-      <c r="BI14" s="58"/>
+      <c r="BA14" s="31"/>
+      <c r="BB14" s="31"/>
+      <c r="BC14" s="31"/>
+      <c r="BD14" s="31"/>
+      <c r="BE14" s="31"/>
+      <c r="BF14" s="31"/>
+      <c r="BG14" s="31"/>
+      <c r="BH14" s="31"/>
+      <c r="BI14" s="31"/>
       <c r="BJ14" s="31"/>
       <c r="BK14" s="31"/>
     </row>
@@ -12491,6 +12487,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="76b82b46-d00a-4f8f-bcd0-332378d7cd39">
@@ -12506,15 +12511,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12537,6 +12533,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA46F6D6-491B-41F7-B12E-75A9D32260DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C90A98FB-4049-4534-8A58-D274716CC406}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12545,12 +12549,4 @@
     <ds:schemaRef ds:uri="1fc22514-bf04-4007-b8f5-80d790464e63"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA46F6D6-491B-41F7-B12E-75A9D32260DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>